<commit_message>
Angular material and bootstrap
</commit_message>
<xml_diff>
--- a/P2 Teams.xlsx
+++ b/P2 Teams.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil Shah\Desktop\training_sessions\rev030722\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3806B5B9-CBF0-4D57-9B77-E3189EB0A0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AE76A2-527F-4171-9A9A-4FD9602159C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6A978434-47F2-4320-A7D8-458D96B57A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Team 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Team 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Team 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Team 4" sheetId="5" r:id="rId5"/>
-    <sheet name="Team 5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
+    <sheet name="Team 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Team 3" sheetId="4" r:id="rId5"/>
+    <sheet name="Team 4" sheetId="5" r:id="rId6"/>
+    <sheet name="Team 5" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$22</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Arthur Leyva</t>
   </si>
@@ -112,6 +113,33 @@
   </si>
   <si>
     <t>JT</t>
+  </si>
+  <si>
+    <t>Team A</t>
+  </si>
+  <si>
+    <t>Typeing Project</t>
+  </si>
+  <si>
+    <t>Team B</t>
+  </si>
+  <si>
+    <t>Trip Planner APP</t>
+  </si>
+  <si>
+    <t>Team C</t>
+  </si>
+  <si>
+    <t>Donation APP</t>
+  </si>
+  <si>
+    <t>Team D</t>
+  </si>
+  <si>
+    <t>Team E</t>
+  </si>
+  <si>
+    <t>TypingDB</t>
   </si>
 </sst>
 </file>
@@ -750,7 +778,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -784,11 +812,67 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C25187-85CA-4BC7-972C-AF6ACF5EAD8D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E677E6B8-4728-4DD6-BC10-3ACDB8A22966}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -818,12 +902,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C709D2-3D72-4005-892D-B21338CC57F4}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -849,21 +933,19 @@
       </c>
     </row>
     <row r="5" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462DC0B7-CB2C-4D68-8CE5-52DEC91D9246}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -879,8 +961,8 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
+      <c r="A3" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -893,12 +975,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7AF2EF-22E6-4A6A-BFDD-17CFA2CDA410}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" activeCellId="3" sqref="A4 A2 A1 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>